<commit_message>
corrected sens and fpr in cross val. and new data
</commit_message>
<xml_diff>
--- a/matlab/final/results/error plot and accuracy.xlsx
+++ b/matlab/final/results/error plot and accuracy.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="12">
   <si>
     <t>Dog 1</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>200,fpr</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -349,11 +352,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-588035808"/>
-        <c:axId val="-627460640"/>
+        <c:axId val="-326380448"/>
+        <c:axId val="-204936448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-588035808"/>
+        <c:axId val="-326380448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -396,7 +399,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-627460640"/>
+        <c:crossAx val="-204936448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -404,7 +407,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-627460640"/>
+        <c:axId val="-204936448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -512,7 +515,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-588035808"/>
+        <c:crossAx val="-326380448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -729,19 +732,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7.0000000000000009</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.6000000000000005</c:v>
+                  <c:v>56.000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5069444444444402</c:v>
+                  <c:v>25.0694444444444</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1169154228855698</c:v>
+                  <c:v>41.143518518518505</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6222222222222196</c:v>
+                  <c:v>36.2222222222222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -801,16 +804,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>98.3333333333333</c:v>
+                  <c:v>86.6666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.1944444444444</c:v>
+                  <c:v>82.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.556701030927798</c:v>
+                  <c:v>85.3333333333334</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>100</c:v>
@@ -829,11 +832,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-588035216"/>
-        <c:axId val="-627464288"/>
+        <c:axId val="-326379856"/>
+        <c:axId val="-204935232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-588035216"/>
+        <c:axId val="-326379856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,7 +879,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-627464288"/>
+        <c:crossAx val="-204935232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -884,7 +887,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-627464288"/>
+        <c:axId val="-204935232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -992,7 +995,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-588035216"/>
+        <c:crossAx val="-326379856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1107,6 +1110,486 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>False Positive Rate and Sensitvity Of 10-Fold Cross Validation Predictions (1000 epochs)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'fpr and sens'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FPR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'fpr and sens'!$I$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Dog 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dog 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dog 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dog 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dog 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'fpr and sens'!$I$10:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.9583333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.865740740740698</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.7777777777778</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'fpr and sens'!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sensitivity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'fpr and sens'!$I$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Dog 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dog 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dog 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dog 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dog 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'fpr and sens'!$I$11:$M$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.142857142857096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.2222222222222</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.6666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-126645872"/>
+        <c:axId val="-207075024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-126645872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-207075024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-207075024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percent</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-126645872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Dog 1 Sensitivity</a:t>
             </a:r>
@@ -3638,11 +4121,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-590993072"/>
-        <c:axId val="-590996720"/>
+        <c:axId val="-204950432"/>
+        <c:axId val="-204934016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-590993072"/>
+        <c:axId val="-204950432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -3756,12 +4239,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-590996720"/>
+        <c:crossAx val="-204934016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-590996720"/>
+        <c:axId val="-204934016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3875,7 +4358,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-590993072"/>
+        <c:crossAx val="-204950432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3956,7 +4439,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -14775,11 +15258,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-627469760"/>
-        <c:axId val="-627463072"/>
+        <c:axId val="-204932800"/>
+        <c:axId val="-204948608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-627469760"/>
+        <c:axId val="-204932800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -14893,12 +15376,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-627463072"/>
+        <c:crossAx val="-204948608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-627463072"/>
+        <c:axId val="-204948608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15016,7 +15499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-627469760"/>
+        <c:crossAx val="-204932800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15218,6 +15701,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -16264,7 +16787,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -16291,8 +16814,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -16393,7 +16916,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -16425,10 +16948,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -16468,23 +16991,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -16589,8 +17111,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -16722,20 +17244,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -16749,17 +17270,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -17295,20 +17805,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17354,6 +18380,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -17695,10 +18753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17722,6 +18780,9 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
       <c r="I1" t="s">
         <v>0</v>
       </c>
@@ -17843,6 +18904,9 @@
       <c r="F5" t="s">
         <v>4</v>
       </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
       <c r="I5" t="s">
         <v>0</v>
       </c>
@@ -17864,42 +18928,42 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>7.0000000000000007E-2</v>
+        <v>0.7</v>
       </c>
       <c r="C6">
-        <v>5.6000000000000001E-2</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D6">
-        <v>2.5069444444444401E-2</v>
+        <v>0.250694444444444</v>
       </c>
       <c r="E6">
-        <v>4.1169154228855698E-2</v>
+        <v>0.41143518518518502</v>
       </c>
       <c r="F6">
-        <v>3.6222222222222197E-2</v>
+        <v>0.362222222222222</v>
       </c>
       <c r="H6" t="s">
         <v>6</v>
       </c>
       <c r="I6">
         <f>B6*100</f>
-        <v>7.0000000000000009</v>
+        <v>70</v>
       </c>
       <c r="J6">
         <f t="shared" ref="J6:J7" si="5">C6*100</f>
-        <v>5.6000000000000005</v>
+        <v>56.000000000000007</v>
       </c>
       <c r="K6">
         <f t="shared" ref="K6:K7" si="6">D6*100</f>
-        <v>2.5069444444444402</v>
+        <v>25.0694444444444</v>
       </c>
       <c r="L6">
         <f t="shared" ref="L6:L7" si="7">E6*100</f>
-        <v>4.1169154228855698</v>
+        <v>41.143518518518505</v>
       </c>
       <c r="M6">
         <f t="shared" ref="M6:M7" si="8">F6*100</f>
-        <v>3.6222222222222196</v>
+        <v>36.2222222222222</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -17907,16 +18971,16 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.98333333333333295</v>
+        <v>0.86666666666666703</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0.98194444444444395</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="E7">
-        <v>0.98556701030927796</v>
+        <v>0.85333333333333405</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -17926,7 +18990,7 @@
       </c>
       <c r="I7">
         <f>B7*100</f>
-        <v>98.3333333333333</v>
+        <v>86.6666666666667</v>
       </c>
       <c r="J7">
         <f t="shared" si="5"/>
@@ -17934,15 +18998,139 @@
       </c>
       <c r="K7">
         <f t="shared" si="6"/>
-        <v>98.1944444444444</v>
+        <v>82.5</v>
       </c>
       <c r="L7">
         <f t="shared" si="7"/>
-        <v>98.556701030927798</v>
+        <v>85.3333333333334</v>
       </c>
       <c r="M7">
         <f t="shared" si="8"/>
         <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1000</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>0.128</v>
+      </c>
+      <c r="C10">
+        <v>0.128</v>
+      </c>
+      <c r="D10">
+        <v>0.33958333333333302</v>
+      </c>
+      <c r="E10">
+        <v>0.218657407407407</v>
+      </c>
+      <c r="F10">
+        <v>0.21777777777777799</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <f>B10*100</f>
+        <v>12.8</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ref="J10:J11" si="9">C10*100</f>
+        <v>12.8</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:K11" si="10">D10*100</f>
+        <v>33.9583333333333</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ref="L10:L11" si="11">E10*100</f>
+        <v>21.865740740740698</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10:M11" si="12">F10*100</f>
+        <v>21.7777777777778</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="C11">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="D11">
+        <v>0.871428571428571</v>
+      </c>
+      <c r="E11">
+        <v>0.74222222222222201</v>
+      </c>
+      <c r="F11">
+        <v>0.96666666666666701</v>
+      </c>
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <f>B11*100</f>
+        <v>97.5</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="9"/>
+        <v>97.5</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="10"/>
+        <v>87.142857142857096</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="11"/>
+        <v>74.2222222222222</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="12"/>
+        <v>96.6666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -20810,7 +21998,7 @@
   <dimension ref="A1:F501"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>